<commit_message>
update code to sample data + change format sample data
</commit_message>
<xml_diff>
--- a/sample_data/data.xlsx
+++ b/sample_data/data.xlsx
@@ -73,6 +73,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -116,13 +119,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E109"/>
+  <dimension ref="A1:E108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E89" sqref="E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -414,20 +420,20 @@
     <col min="2" max="2" width="12.21875" customWidth="1"/>
     <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.77734375" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -447,7 +453,7 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="4">
         <v>42736</v>
       </c>
     </row>
@@ -464,7 +470,7 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="4">
         <v>42767</v>
       </c>
     </row>
@@ -481,7 +487,7 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="4">
         <v>42795</v>
       </c>
     </row>
@@ -498,7 +504,7 @@
       <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="4">
         <v>42826</v>
       </c>
     </row>
@@ -515,7 +521,7 @@
       <c r="D6" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="4">
         <v>42856</v>
       </c>
     </row>
@@ -532,7 +538,7 @@
       <c r="D7" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="4">
         <v>42887</v>
       </c>
     </row>
@@ -549,7 +555,7 @@
       <c r="D8" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="4">
         <v>42917</v>
       </c>
     </row>
@@ -566,7 +572,7 @@
       <c r="D9" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="4">
         <v>42948</v>
       </c>
     </row>
@@ -583,7 +589,7 @@
       <c r="D10" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="4">
         <v>42979</v>
       </c>
     </row>
@@ -600,7 +606,7 @@
       <c r="D11" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="4">
         <v>43009</v>
       </c>
     </row>
@@ -617,7 +623,7 @@
       <c r="D12" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="4">
         <v>43040</v>
       </c>
     </row>
@@ -634,7 +640,7 @@
       <c r="D13" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="4">
         <v>43070</v>
       </c>
     </row>
@@ -651,7 +657,7 @@
       <c r="D14" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="4">
         <v>43101</v>
       </c>
     </row>
@@ -668,7 +674,7 @@
       <c r="D15" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="4">
         <v>43132</v>
       </c>
     </row>
@@ -685,7 +691,7 @@
       <c r="D16" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="4">
         <v>43160</v>
       </c>
     </row>
@@ -702,7 +708,7 @@
       <c r="D17" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="4">
         <v>43191</v>
       </c>
     </row>
@@ -713,13 +719,13 @@
       <c r="B18" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>-41.62</v>
       </c>
       <c r="D18" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="4">
         <v>42738</v>
       </c>
     </row>
@@ -730,13 +736,13 @@
       <c r="B19" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="1">
         <v>-56.45</v>
       </c>
       <c r="D19" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="4">
         <v>42751</v>
       </c>
     </row>
@@ -747,13 +753,13 @@
       <c r="B20" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="1">
         <v>-36.39</v>
       </c>
       <c r="D20" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="4">
         <v>42762</v>
       </c>
     </row>
@@ -764,13 +770,13 @@
       <c r="B21" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="1">
         <v>-50.29</v>
       </c>
       <c r="D21" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="4">
         <v>42781</v>
       </c>
     </row>
@@ -781,13 +787,13 @@
       <c r="B22" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="1">
         <v>-44.55</v>
       </c>
       <c r="D22" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="4">
         <v>42790</v>
       </c>
     </row>
@@ -798,13 +804,13 @@
       <c r="B23" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="1">
         <v>-36.64</v>
       </c>
       <c r="D23" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="4">
         <v>42801</v>
       </c>
     </row>
@@ -815,13 +821,13 @@
       <c r="B24" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="1">
         <v>-38.68</v>
       </c>
       <c r="D24" t="s">
         <v>5</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24" s="4">
         <v>42815</v>
       </c>
     </row>
@@ -832,13 +838,13 @@
       <c r="B25" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="1">
         <v>-33.49</v>
       </c>
       <c r="D25" t="s">
         <v>5</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25" s="4">
         <v>42830</v>
       </c>
     </row>
@@ -849,13 +855,13 @@
       <c r="B26" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="1">
         <v>-44.25</v>
       </c>
       <c r="D26" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26" s="4">
         <v>42841</v>
       </c>
     </row>
@@ -866,13 +872,13 @@
       <c r="B27" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="1">
         <v>-46.46</v>
       </c>
       <c r="D27" t="s">
         <v>5</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E27" s="4">
         <v>42859</v>
       </c>
     </row>
@@ -883,13 +889,13 @@
       <c r="B28" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="1">
         <v>-35.75</v>
       </c>
       <c r="D28" t="s">
         <v>5</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E28" s="4">
         <v>42872</v>
       </c>
     </row>
@@ -900,13 +906,13 @@
       <c r="B29" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="1">
         <v>-53.04</v>
       </c>
       <c r="D29" t="s">
         <v>5</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E29" s="4">
         <v>42884</v>
       </c>
     </row>
@@ -917,13 +923,13 @@
       <c r="B30" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="1">
         <v>-47.7</v>
       </c>
       <c r="D30" t="s">
         <v>5</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E30" s="4">
         <v>42897</v>
       </c>
     </row>
@@ -934,13 +940,13 @@
       <c r="B31" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="1">
         <v>-55.15</v>
       </c>
       <c r="D31" t="s">
         <v>5</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E31" s="4">
         <v>42915</v>
       </c>
     </row>
@@ -951,13 +957,13 @@
       <c r="B32" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="1">
         <v>-58.83</v>
       </c>
       <c r="D32" t="s">
         <v>5</v>
       </c>
-      <c r="E32" s="1">
+      <c r="E32" s="4">
         <v>42925</v>
       </c>
     </row>
@@ -968,13 +974,13 @@
       <c r="B33" t="s">
         <v>10</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="1">
         <v>-55.09</v>
       </c>
       <c r="D33" t="s">
         <v>5</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E33" s="4">
         <v>42943</v>
       </c>
     </row>
@@ -985,13 +991,13 @@
       <c r="B34" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="1">
         <v>-50.15</v>
       </c>
       <c r="D34" t="s">
         <v>5</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E34" s="4">
         <v>42954</v>
       </c>
     </row>
@@ -1002,13 +1008,13 @@
       <c r="B35" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="1">
         <v>-36.5</v>
       </c>
       <c r="D35" t="s">
         <v>5</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E35" s="4">
         <v>42968</v>
       </c>
     </row>
@@ -1019,13 +1025,13 @@
       <c r="B36" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="1">
         <v>-36.909999999999997</v>
       </c>
       <c r="D36" t="s">
         <v>5</v>
       </c>
-      <c r="E36" s="1">
+      <c r="E36" s="4">
         <v>42981</v>
       </c>
     </row>
@@ -1036,13 +1042,13 @@
       <c r="B37" t="s">
         <v>9</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="1">
         <v>-32.31</v>
       </c>
       <c r="D37" t="s">
         <v>5</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E37" s="4">
         <v>43001</v>
       </c>
     </row>
@@ -1053,13 +1059,13 @@
       <c r="B38" t="s">
         <v>10</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="1">
         <v>-36.159999999999997</v>
       </c>
       <c r="D38" t="s">
         <v>5</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E38" s="4">
         <v>43015</v>
       </c>
     </row>
@@ -1070,13 +1076,13 @@
       <c r="B39" t="s">
         <v>10</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="1">
         <v>-41.7</v>
       </c>
       <c r="D39" t="s">
         <v>5</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E39" s="4">
         <v>43031</v>
       </c>
     </row>
@@ -1087,13 +1093,13 @@
       <c r="B40" t="s">
         <v>9</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="1">
         <v>-32.54</v>
       </c>
       <c r="D40" t="s">
         <v>5</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E40" s="4">
         <v>43040</v>
       </c>
     </row>
@@ -1104,13 +1110,13 @@
       <c r="B41" t="s">
         <v>10</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="1">
         <v>-54.99</v>
       </c>
       <c r="D41" t="s">
         <v>5</v>
       </c>
-      <c r="E41" s="1">
+      <c r="E41" s="4">
         <v>43049</v>
       </c>
     </row>
@@ -1121,13 +1127,13 @@
       <c r="B42" t="s">
         <v>9</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="1">
         <v>-46.89</v>
       </c>
       <c r="D42" t="s">
         <v>5</v>
       </c>
-      <c r="E42" s="1">
+      <c r="E42" s="4">
         <v>43065</v>
       </c>
     </row>
@@ -1138,13 +1144,13 @@
       <c r="B43" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="1">
         <v>-41.41</v>
       </c>
       <c r="D43" t="s">
         <v>5</v>
       </c>
-      <c r="E43" s="1">
+      <c r="E43" s="4">
         <v>43072</v>
       </c>
     </row>
@@ -1155,13 +1161,13 @@
       <c r="B44" t="s">
         <v>10</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="1">
         <v>-40.04</v>
       </c>
       <c r="D44" t="s">
         <v>5</v>
       </c>
-      <c r="E44" s="1">
+      <c r="E44" s="4">
         <v>43091</v>
       </c>
     </row>
@@ -1172,13 +1178,13 @@
       <c r="B45" t="s">
         <v>9</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="1">
         <v>-34.53</v>
       </c>
       <c r="D45" t="s">
         <v>5</v>
       </c>
-      <c r="E45" s="1">
+      <c r="E45" s="4">
         <v>43111</v>
       </c>
     </row>
@@ -1189,13 +1195,13 @@
       <c r="B46" t="s">
         <v>10</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="1">
         <v>-42.92</v>
       </c>
       <c r="D46" t="s">
         <v>5</v>
       </c>
-      <c r="E46" s="1">
+      <c r="E46" s="4">
         <v>43126</v>
       </c>
     </row>
@@ -1206,13 +1212,13 @@
       <c r="B47" t="s">
         <v>9</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="1">
         <v>-37.03</v>
       </c>
       <c r="D47" t="s">
         <v>5</v>
       </c>
-      <c r="E47" s="1">
+      <c r="E47" s="4">
         <v>43145</v>
       </c>
     </row>
@@ -1223,13 +1229,13 @@
       <c r="B48" t="s">
         <v>10</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="1">
         <v>-57.3</v>
       </c>
       <c r="D48" t="s">
         <v>5</v>
       </c>
-      <c r="E48" s="1">
+      <c r="E48" s="4">
         <v>43165</v>
       </c>
     </row>
@@ -1240,13 +1246,13 @@
       <c r="B49" t="s">
         <v>9</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="1">
         <v>-48.81</v>
       </c>
       <c r="D49" t="s">
         <v>5</v>
       </c>
-      <c r="E49" s="1">
+      <c r="E49" s="4">
         <v>43185</v>
       </c>
     </row>
@@ -1257,13 +1263,13 @@
       <c r="B50" t="s">
         <v>9</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="1">
         <v>-38.96</v>
       </c>
       <c r="D50" t="s">
         <v>5</v>
       </c>
-      <c r="E50" s="1">
+      <c r="E50" s="4">
         <v>43201</v>
       </c>
     </row>
@@ -1274,13 +1280,13 @@
       <c r="B51" t="s">
         <v>11</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51" s="1">
         <v>-10</v>
       </c>
       <c r="D51" t="s">
         <v>6</v>
       </c>
-      <c r="E51" s="1">
+      <c r="E51" s="4">
         <v>42745</v>
       </c>
     </row>
@@ -1291,13 +1297,13 @@
       <c r="B52" t="s">
         <v>11</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52" s="1">
         <v>-10</v>
       </c>
       <c r="D52" t="s">
         <v>6</v>
       </c>
-      <c r="E52" s="1">
+      <c r="E52" s="4">
         <v>42767</v>
       </c>
     </row>
@@ -1308,13 +1314,13 @@
       <c r="B53" t="s">
         <v>11</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53" s="1">
         <v>-10</v>
       </c>
       <c r="D53" t="s">
         <v>6</v>
       </c>
-      <c r="E53" s="1">
+      <c r="E53" s="4">
         <v>42789</v>
       </c>
     </row>
@@ -1325,13 +1331,13 @@
       <c r="B54" t="s">
         <v>11</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54" s="1">
         <v>-10</v>
       </c>
       <c r="D54" t="s">
         <v>6</v>
       </c>
-      <c r="E54" s="1">
+      <c r="E54" s="4">
         <v>42811</v>
       </c>
     </row>
@@ -1342,13 +1348,13 @@
       <c r="B55" t="s">
         <v>11</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55" s="1">
         <v>-10</v>
       </c>
       <c r="D55" t="s">
         <v>6</v>
       </c>
-      <c r="E55" s="1">
+      <c r="E55" s="4">
         <v>42833</v>
       </c>
     </row>
@@ -1359,13 +1365,13 @@
       <c r="B56" t="s">
         <v>11</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56" s="1">
         <v>-10</v>
       </c>
       <c r="D56" t="s">
         <v>6</v>
       </c>
-      <c r="E56" s="1">
+      <c r="E56" s="4">
         <v>42855</v>
       </c>
     </row>
@@ -1376,13 +1382,13 @@
       <c r="B57" t="s">
         <v>11</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C57" s="1">
         <v>-10</v>
       </c>
       <c r="D57" t="s">
         <v>6</v>
       </c>
-      <c r="E57" s="1">
+      <c r="E57" s="4">
         <v>42877</v>
       </c>
     </row>
@@ -1393,13 +1399,13 @@
       <c r="B58" t="s">
         <v>11</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C58" s="1">
         <v>-10</v>
       </c>
       <c r="D58" t="s">
         <v>6</v>
       </c>
-      <c r="E58" s="1">
+      <c r="E58" s="4">
         <v>42899</v>
       </c>
     </row>
@@ -1410,13 +1416,13 @@
       <c r="B59" t="s">
         <v>11</v>
       </c>
-      <c r="C59" s="2">
+      <c r="C59" s="1">
         <v>-10</v>
       </c>
       <c r="D59" t="s">
         <v>6</v>
       </c>
-      <c r="E59" s="1">
+      <c r="E59" s="4">
         <v>42921</v>
       </c>
     </row>
@@ -1427,13 +1433,13 @@
       <c r="B60" t="s">
         <v>11</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C60" s="1">
         <v>-10</v>
       </c>
       <c r="D60" t="s">
         <v>6</v>
       </c>
-      <c r="E60" s="1">
+      <c r="E60" s="4">
         <v>42943</v>
       </c>
     </row>
@@ -1444,13 +1450,13 @@
       <c r="B61" t="s">
         <v>11</v>
       </c>
-      <c r="C61" s="2">
+      <c r="C61" s="1">
         <v>-10</v>
       </c>
       <c r="D61" t="s">
         <v>6</v>
       </c>
-      <c r="E61" s="1">
+      <c r="E61" s="4">
         <v>42965</v>
       </c>
     </row>
@@ -1461,13 +1467,13 @@
       <c r="B62" t="s">
         <v>11</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C62" s="1">
         <v>-10</v>
       </c>
       <c r="D62" t="s">
         <v>6</v>
       </c>
-      <c r="E62" s="1">
+      <c r="E62" s="4">
         <v>42987</v>
       </c>
     </row>
@@ -1478,13 +1484,13 @@
       <c r="B63" t="s">
         <v>11</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C63" s="1">
         <v>-10</v>
       </c>
       <c r="D63" t="s">
         <v>6</v>
       </c>
-      <c r="E63" s="1">
+      <c r="E63" s="4">
         <v>43009</v>
       </c>
     </row>
@@ -1495,13 +1501,13 @@
       <c r="B64" t="s">
         <v>11</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C64" s="1">
         <v>-10</v>
       </c>
       <c r="D64" t="s">
         <v>6</v>
       </c>
-      <c r="E64" s="1">
+      <c r="E64" s="4">
         <v>43031</v>
       </c>
     </row>
@@ -1512,13 +1518,13 @@
       <c r="B65" t="s">
         <v>11</v>
       </c>
-      <c r="C65" s="2">
+      <c r="C65" s="1">
         <v>-10</v>
       </c>
       <c r="D65" t="s">
         <v>6</v>
       </c>
-      <c r="E65" s="1">
+      <c r="E65" s="4">
         <v>43053</v>
       </c>
     </row>
@@ -1529,13 +1535,13 @@
       <c r="B66" t="s">
         <v>11</v>
       </c>
-      <c r="C66" s="2">
+      <c r="C66" s="1">
         <v>-10</v>
       </c>
       <c r="D66" t="s">
         <v>6</v>
       </c>
-      <c r="E66" s="1">
+      <c r="E66" s="4">
         <v>43075</v>
       </c>
     </row>
@@ -1546,13 +1552,13 @@
       <c r="B67" t="s">
         <v>11</v>
       </c>
-      <c r="C67" s="2">
+      <c r="C67" s="1">
         <v>-10</v>
       </c>
       <c r="D67" t="s">
         <v>6</v>
       </c>
-      <c r="E67" s="1">
+      <c r="E67" s="4">
         <v>43097</v>
       </c>
     </row>
@@ -1563,13 +1569,13 @@
       <c r="B68" t="s">
         <v>11</v>
       </c>
-      <c r="C68" s="2">
+      <c r="C68" s="1">
         <v>-10</v>
       </c>
       <c r="D68" t="s">
         <v>6</v>
       </c>
-      <c r="E68" s="1">
+      <c r="E68" s="4">
         <v>43119</v>
       </c>
     </row>
@@ -1580,13 +1586,13 @@
       <c r="B69" t="s">
         <v>11</v>
       </c>
-      <c r="C69" s="2">
+      <c r="C69" s="1">
         <v>-10</v>
       </c>
       <c r="D69" t="s">
         <v>6</v>
       </c>
-      <c r="E69" s="1">
+      <c r="E69" s="4">
         <v>43141</v>
       </c>
     </row>
@@ -1597,13 +1603,13 @@
       <c r="B70" t="s">
         <v>11</v>
       </c>
-      <c r="C70" s="2">
+      <c r="C70" s="1">
         <v>-10</v>
       </c>
       <c r="D70" t="s">
         <v>6</v>
       </c>
-      <c r="E70" s="1">
+      <c r="E70" s="4">
         <v>43163</v>
       </c>
     </row>
@@ -1614,13 +1620,13 @@
       <c r="B71" t="s">
         <v>11</v>
       </c>
-      <c r="C71" s="2">
+      <c r="C71" s="1">
         <v>-10</v>
       </c>
       <c r="D71" t="s">
         <v>6</v>
       </c>
-      <c r="E71" s="1">
+      <c r="E71" s="4">
         <v>43185</v>
       </c>
     </row>
@@ -1628,13 +1634,13 @@
       <c r="A72">
         <v>71</v>
       </c>
-      <c r="C72" s="2">
+      <c r="C72" s="1">
         <v>1200</v>
       </c>
       <c r="D72" t="s">
         <v>12</v>
       </c>
-      <c r="E72" s="1">
+      <c r="E72" s="4">
         <v>42736</v>
       </c>
     </row>
@@ -1642,13 +1648,13 @@
       <c r="A73">
         <v>72</v>
       </c>
-      <c r="C73" s="2">
+      <c r="C73" s="1">
         <v>1200</v>
       </c>
       <c r="D73" t="s">
         <v>12</v>
       </c>
-      <c r="E73" s="1">
+      <c r="E73" s="4">
         <v>42767</v>
       </c>
     </row>
@@ -1656,13 +1662,13 @@
       <c r="A74">
         <v>73</v>
       </c>
-      <c r="C74" s="2">
+      <c r="C74" s="1">
         <v>1200</v>
       </c>
       <c r="D74" t="s">
         <v>12</v>
       </c>
-      <c r="E74" s="1">
+      <c r="E74" s="4">
         <v>42795</v>
       </c>
     </row>
@@ -1670,13 +1676,13 @@
       <c r="A75">
         <v>74</v>
       </c>
-      <c r="C75" s="2">
+      <c r="C75" s="1">
         <v>1200</v>
       </c>
       <c r="D75" t="s">
         <v>12</v>
       </c>
-      <c r="E75" s="1">
+      <c r="E75" s="4">
         <v>42826</v>
       </c>
     </row>
@@ -1684,13 +1690,13 @@
       <c r="A76">
         <v>75</v>
       </c>
-      <c r="C76" s="2">
+      <c r="C76" s="1">
         <v>1200</v>
       </c>
       <c r="D76" t="s">
         <v>12</v>
       </c>
-      <c r="E76" s="1">
+      <c r="E76" s="4">
         <v>42856</v>
       </c>
     </row>
@@ -1698,13 +1704,13 @@
       <c r="A77">
         <v>76</v>
       </c>
-      <c r="C77" s="2">
+      <c r="C77" s="1">
         <v>1200</v>
       </c>
       <c r="D77" t="s">
         <v>12</v>
       </c>
-      <c r="E77" s="1">
+      <c r="E77" s="4">
         <v>42887</v>
       </c>
     </row>
@@ -1712,13 +1718,13 @@
       <c r="A78">
         <v>77</v>
       </c>
-      <c r="C78" s="2">
+      <c r="C78" s="1">
         <v>1200</v>
       </c>
       <c r="D78" t="s">
         <v>12</v>
       </c>
-      <c r="E78" s="1">
+      <c r="E78" s="4">
         <v>42917</v>
       </c>
     </row>
@@ -1726,13 +1732,13 @@
       <c r="A79">
         <v>78</v>
       </c>
-      <c r="C79" s="2">
+      <c r="C79" s="1">
         <v>1200</v>
       </c>
       <c r="D79" t="s">
         <v>12</v>
       </c>
-      <c r="E79" s="1">
+      <c r="E79" s="4">
         <v>42948</v>
       </c>
     </row>
@@ -1740,13 +1746,13 @@
       <c r="A80">
         <v>79</v>
       </c>
-      <c r="C80" s="2">
+      <c r="C80" s="1">
         <v>1200</v>
       </c>
       <c r="D80" t="s">
         <v>12</v>
       </c>
-      <c r="E80" s="1">
+      <c r="E80" s="4">
         <v>42979</v>
       </c>
     </row>
@@ -1754,13 +1760,13 @@
       <c r="A81">
         <v>80</v>
       </c>
-      <c r="C81" s="2">
+      <c r="C81" s="1">
         <v>1200</v>
       </c>
       <c r="D81" t="s">
         <v>12</v>
       </c>
-      <c r="E81" s="1">
+      <c r="E81" s="4">
         <v>43009</v>
       </c>
     </row>
@@ -1768,13 +1774,13 @@
       <c r="A82">
         <v>81</v>
       </c>
-      <c r="C82" s="2">
+      <c r="C82" s="1">
         <v>1200</v>
       </c>
       <c r="D82" t="s">
         <v>12</v>
       </c>
-      <c r="E82" s="1">
+      <c r="E82" s="4">
         <v>43040</v>
       </c>
     </row>
@@ -1782,13 +1788,13 @@
       <c r="A83">
         <v>82</v>
       </c>
-      <c r="C83" s="2">
+      <c r="C83" s="1">
         <v>1200</v>
       </c>
       <c r="D83" t="s">
         <v>12</v>
       </c>
-      <c r="E83" s="1">
+      <c r="E83" s="4">
         <v>43070</v>
       </c>
     </row>
@@ -1796,13 +1802,13 @@
       <c r="A84">
         <v>83</v>
       </c>
-      <c r="C84" s="2">
+      <c r="C84" s="1">
         <v>1200</v>
       </c>
       <c r="D84" t="s">
         <v>12</v>
       </c>
-      <c r="E84" s="1">
+      <c r="E84" s="4">
         <v>43101</v>
       </c>
     </row>
@@ -1810,13 +1816,13 @@
       <c r="A85">
         <v>84</v>
       </c>
-      <c r="C85" s="2">
+      <c r="C85" s="1">
         <v>1200</v>
       </c>
       <c r="D85" t="s">
         <v>12</v>
       </c>
-      <c r="E85" s="1">
+      <c r="E85" s="4">
         <v>43132</v>
       </c>
     </row>
@@ -1824,13 +1830,13 @@
       <c r="A86">
         <v>85</v>
       </c>
-      <c r="C86" s="2">
+      <c r="C86" s="1">
         <v>1200</v>
       </c>
       <c r="D86" t="s">
         <v>12</v>
       </c>
-      <c r="E86" s="1">
+      <c r="E86" s="4">
         <v>43160</v>
       </c>
     </row>
@@ -1838,13 +1844,13 @@
       <c r="A87">
         <v>86</v>
       </c>
-      <c r="C87" s="2">
+      <c r="C87" s="1">
         <v>1200</v>
       </c>
       <c r="D87" t="s">
         <v>12</v>
       </c>
-      <c r="E87" s="1">
+      <c r="E87" s="4">
         <v>43191</v>
       </c>
     </row>
@@ -1852,14 +1858,14 @@
       <c r="A88">
         <v>87</v>
       </c>
-      <c r="C88" s="2">
+      <c r="C88" s="1">
         <v>200</v>
       </c>
       <c r="D88" t="s">
         <v>13</v>
       </c>
-      <c r="E88" s="1">
-        <v>43459</v>
+      <c r="E88" s="4">
+        <v>43094</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
@@ -1875,7 +1881,7 @@
       <c r="D89" t="s">
         <v>6</v>
       </c>
-      <c r="E89" s="1">
+      <c r="E89" s="4">
         <v>42750</v>
       </c>
     </row>
@@ -1892,7 +1898,7 @@
       <c r="D90" t="s">
         <v>6</v>
       </c>
-      <c r="E90" s="1">
+      <c r="E90" s="4">
         <v>42776</v>
       </c>
     </row>
@@ -1909,7 +1915,7 @@
       <c r="D91" t="s">
         <v>6</v>
       </c>
-      <c r="E91" s="1">
+      <c r="E91" s="4">
         <v>42783</v>
       </c>
     </row>
@@ -1926,7 +1932,7 @@
       <c r="D92" t="s">
         <v>6</v>
       </c>
-      <c r="E92" s="1">
+      <c r="E92" s="4">
         <v>42814</v>
       </c>
     </row>
@@ -1943,7 +1949,7 @@
       <c r="D93" t="s">
         <v>6</v>
       </c>
-      <c r="E93" s="1">
+      <c r="E93" s="4">
         <v>42821</v>
       </c>
     </row>
@@ -1960,7 +1966,7 @@
       <c r="D94" t="s">
         <v>6</v>
       </c>
-      <c r="E94" s="1">
+      <c r="E94" s="4">
         <v>42843</v>
       </c>
     </row>
@@ -1977,7 +1983,7 @@
       <c r="D95" t="s">
         <v>6</v>
       </c>
-      <c r="E95" s="1">
+      <c r="E95" s="4">
         <v>42878</v>
       </c>
     </row>
@@ -1994,7 +2000,7 @@
       <c r="D96" t="s">
         <v>6</v>
       </c>
-      <c r="E96" s="1">
+      <c r="E96" s="4">
         <v>42906</v>
       </c>
     </row>
@@ -2011,7 +2017,7 @@
       <c r="D97" t="s">
         <v>6</v>
       </c>
-      <c r="E97" s="1">
+      <c r="E97" s="4">
         <v>42945</v>
       </c>
     </row>
@@ -2028,7 +2034,7 @@
       <c r="D98" t="s">
         <v>6</v>
       </c>
-      <c r="E98" s="1">
+      <c r="E98" s="4">
         <v>42956</v>
       </c>
     </row>
@@ -2045,7 +2051,7 @@
       <c r="D99" t="s">
         <v>6</v>
       </c>
-      <c r="E99" s="1">
+      <c r="E99" s="4">
         <v>42983</v>
       </c>
     </row>
@@ -2062,7 +2068,7 @@
       <c r="D100" t="s">
         <v>6</v>
       </c>
-      <c r="E100" s="1">
+      <c r="E100" s="4">
         <v>43019</v>
       </c>
     </row>
@@ -2079,7 +2085,7 @@
       <c r="D101" t="s">
         <v>6</v>
       </c>
-      <c r="E101" s="1">
+      <c r="E101" s="4">
         <v>43038</v>
       </c>
     </row>
@@ -2096,7 +2102,7 @@
       <c r="D102" t="s">
         <v>6</v>
       </c>
-      <c r="E102" s="1">
+      <c r="E102" s="4">
         <v>43057</v>
       </c>
     </row>
@@ -2113,7 +2119,7 @@
       <c r="D103" t="s">
         <v>6</v>
       </c>
-      <c r="E103" s="1">
+      <c r="E103" s="4">
         <v>43072</v>
       </c>
     </row>
@@ -2130,7 +2136,7 @@
       <c r="D104" t="s">
         <v>6</v>
       </c>
-      <c r="E104" s="1">
+      <c r="E104" s="4">
         <v>43093</v>
       </c>
     </row>
@@ -2147,7 +2153,7 @@
       <c r="D105" t="s">
         <v>6</v>
       </c>
-      <c r="E105" s="1">
+      <c r="E105" s="4">
         <v>43132</v>
       </c>
     </row>
@@ -2164,7 +2170,7 @@
       <c r="D106" t="s">
         <v>6</v>
       </c>
-      <c r="E106" s="1">
+      <c r="E106" s="4">
         <v>43147</v>
       </c>
     </row>
@@ -2181,7 +2187,7 @@
       <c r="D107" t="s">
         <v>6</v>
       </c>
-      <c r="E107" s="1">
+      <c r="E107" s="4">
         <v>43161</v>
       </c>
     </row>
@@ -2198,12 +2204,9 @@
       <c r="D108" t="s">
         <v>6</v>
       </c>
-      <c r="E108" s="1">
+      <c r="E108" s="4">
         <v>43200</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E109" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E109"/>

</xml_diff>

<commit_message>
implement first plot + fix sample data
</commit_message>
<xml_diff>
--- a/sample_data/data.xlsx
+++ b/sample_data/data.xlsx
@@ -411,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E89" sqref="E89"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="F67" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1876,7 +1876,7 @@
         <v>14</v>
       </c>
       <c r="C89">
-        <v>24</v>
+        <v>-24</v>
       </c>
       <c r="D89" t="s">
         <v>6</v>
@@ -1893,7 +1893,7 @@
         <v>14</v>
       </c>
       <c r="C90">
-        <v>30</v>
+        <v>-30</v>
       </c>
       <c r="D90" t="s">
         <v>6</v>
@@ -1910,7 +1910,7 @@
         <v>14</v>
       </c>
       <c r="C91">
-        <v>16</v>
+        <v>-16</v>
       </c>
       <c r="D91" t="s">
         <v>6</v>
@@ -1927,7 +1927,7 @@
         <v>14</v>
       </c>
       <c r="C92">
-        <v>11</v>
+        <v>-11</v>
       </c>
       <c r="D92" t="s">
         <v>6</v>
@@ -1944,7 +1944,7 @@
         <v>14</v>
       </c>
       <c r="C93">
-        <v>37</v>
+        <v>-37</v>
       </c>
       <c r="D93" t="s">
         <v>6</v>
@@ -1961,7 +1961,7 @@
         <v>14</v>
       </c>
       <c r="C94">
-        <v>22</v>
+        <v>-22</v>
       </c>
       <c r="D94" t="s">
         <v>6</v>
@@ -1978,7 +1978,7 @@
         <v>14</v>
       </c>
       <c r="C95">
-        <v>27</v>
+        <v>-27</v>
       </c>
       <c r="D95" t="s">
         <v>6</v>
@@ -1995,7 +1995,7 @@
         <v>14</v>
       </c>
       <c r="C96">
-        <v>32</v>
+        <v>-32</v>
       </c>
       <c r="D96" t="s">
         <v>6</v>
@@ -2012,7 +2012,7 @@
         <v>14</v>
       </c>
       <c r="C97">
-        <v>43</v>
+        <v>-43</v>
       </c>
       <c r="D97" t="s">
         <v>6</v>
@@ -2029,7 +2029,7 @@
         <v>14</v>
       </c>
       <c r="C98">
-        <v>18</v>
+        <v>-18</v>
       </c>
       <c r="D98" t="s">
         <v>6</v>
@@ -2046,7 +2046,7 @@
         <v>14</v>
       </c>
       <c r="C99">
-        <v>19</v>
+        <v>-19</v>
       </c>
       <c r="D99" t="s">
         <v>6</v>
@@ -2063,7 +2063,7 @@
         <v>14</v>
       </c>
       <c r="C100">
-        <v>19</v>
+        <v>-19</v>
       </c>
       <c r="D100" t="s">
         <v>6</v>
@@ -2080,7 +2080,7 @@
         <v>14</v>
       </c>
       <c r="C101">
-        <v>13</v>
+        <v>-13</v>
       </c>
       <c r="D101" t="s">
         <v>6</v>
@@ -2097,7 +2097,7 @@
         <v>14</v>
       </c>
       <c r="C102">
-        <v>23</v>
+        <v>-23</v>
       </c>
       <c r="D102" t="s">
         <v>6</v>
@@ -2114,7 +2114,7 @@
         <v>14</v>
       </c>
       <c r="C103">
-        <v>22</v>
+        <v>-22</v>
       </c>
       <c r="D103" t="s">
         <v>6</v>
@@ -2131,7 +2131,7 @@
         <v>14</v>
       </c>
       <c r="C104">
-        <v>35</v>
+        <v>-35</v>
       </c>
       <c r="D104" t="s">
         <v>6</v>
@@ -2148,7 +2148,7 @@
         <v>14</v>
       </c>
       <c r="C105">
-        <v>38</v>
+        <v>-38</v>
       </c>
       <c r="D105" t="s">
         <v>6</v>
@@ -2165,7 +2165,7 @@
         <v>14</v>
       </c>
       <c r="C106">
-        <v>48</v>
+        <v>-48</v>
       </c>
       <c r="D106" t="s">
         <v>6</v>
@@ -2182,7 +2182,7 @@
         <v>14</v>
       </c>
       <c r="C107">
-        <v>13</v>
+        <v>-13</v>
       </c>
       <c r="D107" t="s">
         <v>6</v>
@@ -2199,7 +2199,7 @@
         <v>14</v>
       </c>
       <c r="C108">
-        <v>10</v>
+        <v>-10</v>
       </c>
       <c r="D108" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
[NEW] sample date improved
</commit_message>
<xml_diff>
--- a/sample_data/data.xlsx
+++ b/sample_data/data.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$E$109</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$E$110</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -68,6 +68,69 @@
   <si>
     <t>Fuel</t>
   </si>
+  <si>
+    <t>Shopping</t>
+  </si>
+  <si>
+    <t>LG G6</t>
+  </si>
+  <si>
+    <t>Games</t>
+  </si>
+  <si>
+    <t>Bills</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>Internet + phone</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>Gym</t>
+  </si>
+  <si>
+    <t>Drugs</t>
+  </si>
+  <si>
+    <t>Travel</t>
+  </si>
+  <si>
+    <t>Weekend</t>
+  </si>
+  <si>
+    <t>Holidays</t>
+  </si>
+  <si>
+    <t>Clothes</t>
+  </si>
+  <si>
+    <t>Motobike repair</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>Fine</t>
+  </si>
+  <si>
+    <t>Taxes</t>
+  </si>
+  <si>
+    <t>Christmas presents</t>
+  </si>
+  <si>
+    <t>TV</t>
+  </si>
+  <si>
+    <t>Motobike</t>
+  </si>
 </sst>
 </file>
 
@@ -76,7 +139,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +149,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -119,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -129,6 +200,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,15 +482,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E108"/>
+  <dimension ref="A1:E200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="F67" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="D201" sqref="D201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.21875" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.77734375" customWidth="1"/>
     <col min="5" max="5" width="11.5546875" style="4" customWidth="1"/>
@@ -1635,7 +1708,7 @@
         <v>71</v>
       </c>
       <c r="C72" s="1">
-        <v>1200</v>
+        <v>1150</v>
       </c>
       <c r="D72" t="s">
         <v>12</v>
@@ -1649,7 +1722,7 @@
         <v>72</v>
       </c>
       <c r="C73" s="1">
-        <v>1200</v>
+        <v>1250</v>
       </c>
       <c r="D73" t="s">
         <v>12</v>
@@ -1691,7 +1764,7 @@
         <v>75</v>
       </c>
       <c r="C76" s="1">
-        <v>1200</v>
+        <v>1250</v>
       </c>
       <c r="D76" t="s">
         <v>12</v>
@@ -1705,7 +1778,7 @@
         <v>76</v>
       </c>
       <c r="C77" s="1">
-        <v>1200</v>
+        <v>1100</v>
       </c>
       <c r="D77" t="s">
         <v>12</v>
@@ -1733,7 +1806,7 @@
         <v>78</v>
       </c>
       <c r="C79" s="1">
-        <v>1200</v>
+        <v>1280</v>
       </c>
       <c r="D79" t="s">
         <v>12</v>
@@ -1747,7 +1820,7 @@
         <v>79</v>
       </c>
       <c r="C80" s="1">
-        <v>1200</v>
+        <v>1300</v>
       </c>
       <c r="D80" t="s">
         <v>12</v>
@@ -1761,7 +1834,7 @@
         <v>80</v>
       </c>
       <c r="C81" s="1">
-        <v>1200</v>
+        <v>1305</v>
       </c>
       <c r="D81" t="s">
         <v>12</v>
@@ -1775,7 +1848,7 @@
         <v>81</v>
       </c>
       <c r="C82" s="1">
-        <v>1200</v>
+        <v>1350</v>
       </c>
       <c r="D82" t="s">
         <v>12</v>
@@ -1789,7 +1862,7 @@
         <v>82</v>
       </c>
       <c r="C83" s="1">
-        <v>1200</v>
+        <v>1340</v>
       </c>
       <c r="D83" t="s">
         <v>12</v>
@@ -1803,7 +1876,7 @@
         <v>83</v>
       </c>
       <c r="C84" s="1">
-        <v>1200</v>
+        <v>1380</v>
       </c>
       <c r="D84" t="s">
         <v>12</v>
@@ -1817,7 +1890,7 @@
         <v>84</v>
       </c>
       <c r="C85" s="1">
-        <v>1200</v>
+        <v>1300</v>
       </c>
       <c r="D85" t="s">
         <v>12</v>
@@ -1831,7 +1904,7 @@
         <v>85</v>
       </c>
       <c r="C86" s="1">
-        <v>1200</v>
+        <v>1350</v>
       </c>
       <c r="D86" t="s">
         <v>12</v>
@@ -1845,7 +1918,7 @@
         <v>86</v>
       </c>
       <c r="C87" s="1">
-        <v>1200</v>
+        <v>1330</v>
       </c>
       <c r="D87" t="s">
         <v>12</v>
@@ -1865,199 +1938,196 @@
         <v>13</v>
       </c>
       <c r="E88" s="4">
-        <v>43094</v>
+        <v>42972</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89">
-        <v>88</v>
-      </c>
-      <c r="B89" t="s">
-        <v>14</v>
-      </c>
-      <c r="C89">
-        <v>-24</v>
+        <v>87</v>
+      </c>
+      <c r="C89" s="1">
+        <v>200</v>
       </c>
       <c r="D89" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E89" s="4">
-        <v>42750</v>
+        <v>43094</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B90" t="s">
         <v>14</v>
       </c>
       <c r="C90">
-        <v>-30</v>
+        <v>-24</v>
       </c>
       <c r="D90" t="s">
         <v>6</v>
       </c>
       <c r="E90" s="4">
-        <v>42776</v>
+        <v>42750</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B91" t="s">
         <v>14</v>
       </c>
       <c r="C91">
-        <v>-16</v>
+        <v>-30</v>
       </c>
       <c r="D91" t="s">
         <v>6</v>
       </c>
       <c r="E91" s="4">
-        <v>42783</v>
+        <v>42776</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B92" t="s">
         <v>14</v>
       </c>
       <c r="C92">
-        <v>-11</v>
+        <v>-16</v>
       </c>
       <c r="D92" t="s">
         <v>6</v>
       </c>
       <c r="E92" s="4">
-        <v>42814</v>
+        <v>42783</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B93" t="s">
         <v>14</v>
       </c>
       <c r="C93">
-        <v>-37</v>
+        <v>-11</v>
       </c>
       <c r="D93" t="s">
         <v>6</v>
       </c>
       <c r="E93" s="4">
-        <v>42821</v>
+        <v>42814</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B94" t="s">
         <v>14</v>
       </c>
       <c r="C94">
-        <v>-22</v>
+        <v>-37</v>
       </c>
       <c r="D94" t="s">
         <v>6</v>
       </c>
       <c r="E94" s="4">
-        <v>42843</v>
+        <v>42821</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B95" t="s">
         <v>14</v>
       </c>
       <c r="C95">
-        <v>-27</v>
+        <v>-22</v>
       </c>
       <c r="D95" t="s">
         <v>6</v>
       </c>
       <c r="E95" s="4">
-        <v>42878</v>
+        <v>42843</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B96" t="s">
         <v>14</v>
       </c>
       <c r="C96">
-        <v>-32</v>
+        <v>-27</v>
       </c>
       <c r="D96" t="s">
         <v>6</v>
       </c>
       <c r="E96" s="4">
-        <v>42906</v>
+        <v>42878</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B97" t="s">
         <v>14</v>
       </c>
       <c r="C97">
-        <v>-43</v>
+        <v>-32</v>
       </c>
       <c r="D97" t="s">
         <v>6</v>
       </c>
       <c r="E97" s="4">
-        <v>42945</v>
+        <v>42906</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B98" t="s">
         <v>14</v>
       </c>
       <c r="C98">
-        <v>-18</v>
+        <v>-43</v>
       </c>
       <c r="D98" t="s">
         <v>6</v>
       </c>
       <c r="E98" s="4">
-        <v>42956</v>
+        <v>42945</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B99" t="s">
         <v>14</v>
       </c>
       <c r="C99">
-        <v>-19</v>
+        <v>-18</v>
       </c>
       <c r="D99" t="s">
         <v>6</v>
       </c>
       <c r="E99" s="4">
-        <v>42983</v>
+        <v>42956</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B100" t="s">
         <v>14</v>
@@ -2069,147 +2139,1680 @@
         <v>6</v>
       </c>
       <c r="E100" s="4">
-        <v>43019</v>
+        <v>42983</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B101" t="s">
         <v>14</v>
       </c>
       <c r="C101">
-        <v>-13</v>
+        <v>-19</v>
       </c>
       <c r="D101" t="s">
         <v>6</v>
       </c>
       <c r="E101" s="4">
-        <v>43038</v>
+        <v>43019</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B102" t="s">
         <v>14</v>
       </c>
       <c r="C102">
-        <v>-23</v>
+        <v>-13</v>
       </c>
       <c r="D102" t="s">
         <v>6</v>
       </c>
       <c r="E102" s="4">
-        <v>43057</v>
+        <v>43038</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B103" t="s">
         <v>14</v>
       </c>
       <c r="C103">
-        <v>-22</v>
+        <v>-23</v>
       </c>
       <c r="D103" t="s">
         <v>6</v>
       </c>
       <c r="E103" s="4">
-        <v>43072</v>
+        <v>43057</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B104" t="s">
         <v>14</v>
       </c>
       <c r="C104">
-        <v>-35</v>
+        <v>-22</v>
       </c>
       <c r="D104" t="s">
         <v>6</v>
       </c>
       <c r="E104" s="4">
-        <v>43093</v>
+        <v>43072</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B105" t="s">
         <v>14</v>
       </c>
       <c r="C105">
-        <v>-38</v>
+        <v>-35</v>
       </c>
       <c r="D105" t="s">
         <v>6</v>
       </c>
       <c r="E105" s="4">
-        <v>43132</v>
+        <v>43093</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B106" t="s">
         <v>14</v>
       </c>
       <c r="C106">
-        <v>-48</v>
+        <v>-38</v>
       </c>
       <c r="D106" t="s">
         <v>6</v>
       </c>
       <c r="E106" s="4">
-        <v>43147</v>
+        <v>43132</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B107" t="s">
         <v>14</v>
       </c>
       <c r="C107">
-        <v>-13</v>
+        <v>-48</v>
       </c>
       <c r="D107" t="s">
         <v>6</v>
       </c>
       <c r="E107" s="4">
-        <v>43161</v>
+        <v>43147</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B108" t="s">
         <v>14</v>
       </c>
       <c r="C108">
+        <v>-13</v>
+      </c>
+      <c r="D108" t="s">
+        <v>6</v>
+      </c>
+      <c r="E108" s="4">
+        <v>43161</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>107</v>
+      </c>
+      <c r="B109" t="s">
+        <v>14</v>
+      </c>
+      <c r="C109">
         <v>-10</v>
       </c>
-      <c r="D108" t="s">
-        <v>6</v>
-      </c>
-      <c r="E108" s="4">
+      <c r="D109" t="s">
+        <v>6</v>
+      </c>
+      <c r="E109" s="4">
         <v>43200</v>
       </c>
     </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>108</v>
+      </c>
+      <c r="B110" t="s">
+        <v>16</v>
+      </c>
+      <c r="C110">
+        <v>-400</v>
+      </c>
+      <c r="D110" t="s">
+        <v>15</v>
+      </c>
+      <c r="E110" s="4">
+        <v>43089</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>109</v>
+      </c>
+      <c r="B111" t="s">
+        <v>17</v>
+      </c>
+      <c r="C111">
+        <v>-50</v>
+      </c>
+      <c r="D111" t="s">
+        <v>15</v>
+      </c>
+      <c r="E111" s="4">
+        <v>42907</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>110</v>
+      </c>
+      <c r="B112" t="s">
+        <v>19</v>
+      </c>
+      <c r="C112">
+        <v>-46</v>
+      </c>
+      <c r="D112" t="s">
+        <v>18</v>
+      </c>
+      <c r="E112" s="4">
+        <v>42736</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>111</v>
+      </c>
+      <c r="B113" t="s">
+        <v>19</v>
+      </c>
+      <c r="C113">
+        <v>-59</v>
+      </c>
+      <c r="D113" t="s">
+        <v>18</v>
+      </c>
+      <c r="E113" s="4">
+        <v>42767</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>112</v>
+      </c>
+      <c r="B114" t="s">
+        <v>19</v>
+      </c>
+      <c r="C114">
+        <v>-57</v>
+      </c>
+      <c r="D114" t="s">
+        <v>18</v>
+      </c>
+      <c r="E114" s="4">
+        <v>42795</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>113</v>
+      </c>
+      <c r="B115" t="s">
+        <v>19</v>
+      </c>
+      <c r="C115">
+        <v>-63</v>
+      </c>
+      <c r="D115" t="s">
+        <v>18</v>
+      </c>
+      <c r="E115" s="4">
+        <v>42826</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>114</v>
+      </c>
+      <c r="B116" t="s">
+        <v>19</v>
+      </c>
+      <c r="C116">
+        <v>-70</v>
+      </c>
+      <c r="D116" t="s">
+        <v>18</v>
+      </c>
+      <c r="E116" s="4">
+        <v>42856</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>115</v>
+      </c>
+      <c r="B117" t="s">
+        <v>19</v>
+      </c>
+      <c r="C117">
+        <v>-68</v>
+      </c>
+      <c r="D117" t="s">
+        <v>18</v>
+      </c>
+      <c r="E117" s="4">
+        <v>42887</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <v>116</v>
+      </c>
+      <c r="B118" t="s">
+        <v>19</v>
+      </c>
+      <c r="C118">
+        <v>-53</v>
+      </c>
+      <c r="D118" t="s">
+        <v>18</v>
+      </c>
+      <c r="E118" s="4">
+        <v>42917</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>117</v>
+      </c>
+      <c r="B119" t="s">
+        <v>19</v>
+      </c>
+      <c r="C119">
+        <v>-62</v>
+      </c>
+      <c r="D119" t="s">
+        <v>18</v>
+      </c>
+      <c r="E119" s="4">
+        <v>42948</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>118</v>
+      </c>
+      <c r="B120" t="s">
+        <v>19</v>
+      </c>
+      <c r="C120">
+        <v>-68</v>
+      </c>
+      <c r="D120" t="s">
+        <v>18</v>
+      </c>
+      <c r="E120" s="4">
+        <v>42979</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <v>119</v>
+      </c>
+      <c r="B121" t="s">
+        <v>19</v>
+      </c>
+      <c r="C121">
+        <v>-58</v>
+      </c>
+      <c r="D121" t="s">
+        <v>18</v>
+      </c>
+      <c r="E121" s="4">
+        <v>43009</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <v>120</v>
+      </c>
+      <c r="B122" t="s">
+        <v>19</v>
+      </c>
+      <c r="C122">
+        <v>-66</v>
+      </c>
+      <c r="D122" t="s">
+        <v>18</v>
+      </c>
+      <c r="E122" s="4">
+        <v>43040</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <v>121</v>
+      </c>
+      <c r="B123" t="s">
+        <v>19</v>
+      </c>
+      <c r="C123">
+        <v>-61</v>
+      </c>
+      <c r="D123" t="s">
+        <v>18</v>
+      </c>
+      <c r="E123" s="4">
+        <v>43070</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <v>122</v>
+      </c>
+      <c r="B124" t="s">
+        <v>19</v>
+      </c>
+      <c r="C124">
+        <v>-59</v>
+      </c>
+      <c r="D124" t="s">
+        <v>18</v>
+      </c>
+      <c r="E124" s="4">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <v>123</v>
+      </c>
+      <c r="B125" t="s">
+        <v>19</v>
+      </c>
+      <c r="C125">
+        <v>-66</v>
+      </c>
+      <c r="D125" t="s">
+        <v>18</v>
+      </c>
+      <c r="E125" s="4">
+        <v>43132</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A126">
+        <v>124</v>
+      </c>
+      <c r="B126" t="s">
+        <v>19</v>
+      </c>
+      <c r="C126">
+        <v>-68</v>
+      </c>
+      <c r="D126" t="s">
+        <v>18</v>
+      </c>
+      <c r="E126" s="4">
+        <v>43160</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <v>125</v>
+      </c>
+      <c r="B127" t="s">
+        <v>19</v>
+      </c>
+      <c r="C127">
+        <v>-43</v>
+      </c>
+      <c r="D127" t="s">
+        <v>18</v>
+      </c>
+      <c r="E127" s="4">
+        <v>43191</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <v>126</v>
+      </c>
+      <c r="B128" t="s">
+        <v>20</v>
+      </c>
+      <c r="C128">
+        <v>-52</v>
+      </c>
+      <c r="D128" t="s">
+        <v>18</v>
+      </c>
+      <c r="E128" s="4">
+        <v>42736</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <v>127</v>
+      </c>
+      <c r="B129" t="s">
+        <v>20</v>
+      </c>
+      <c r="C129">
+        <v>-51</v>
+      </c>
+      <c r="D129" t="s">
+        <v>18</v>
+      </c>
+      <c r="E129" s="4">
+        <v>42767</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <v>128</v>
+      </c>
+      <c r="B130" t="s">
+        <v>20</v>
+      </c>
+      <c r="C130">
+        <v>-50</v>
+      </c>
+      <c r="D130" t="s">
+        <v>18</v>
+      </c>
+      <c r="E130" s="4">
+        <v>42795</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A131">
+        <v>129</v>
+      </c>
+      <c r="B131" t="s">
+        <v>20</v>
+      </c>
+      <c r="C131">
+        <v>-49</v>
+      </c>
+      <c r="D131" t="s">
+        <v>18</v>
+      </c>
+      <c r="E131" s="4">
+        <v>42826</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A132">
+        <v>130</v>
+      </c>
+      <c r="B132" t="s">
+        <v>20</v>
+      </c>
+      <c r="C132">
+        <v>-48</v>
+      </c>
+      <c r="D132" t="s">
+        <v>18</v>
+      </c>
+      <c r="E132" s="4">
+        <v>42856</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A133">
+        <v>131</v>
+      </c>
+      <c r="B133" t="s">
+        <v>20</v>
+      </c>
+      <c r="C133">
+        <v>-47</v>
+      </c>
+      <c r="D133" t="s">
+        <v>18</v>
+      </c>
+      <c r="E133" s="4">
+        <v>42887</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A134">
+        <v>132</v>
+      </c>
+      <c r="B134" t="s">
+        <v>20</v>
+      </c>
+      <c r="C134">
+        <v>-46</v>
+      </c>
+      <c r="D134" t="s">
+        <v>18</v>
+      </c>
+      <c r="E134" s="4">
+        <v>42917</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A135">
+        <v>133</v>
+      </c>
+      <c r="B135" t="s">
+        <v>20</v>
+      </c>
+      <c r="C135">
+        <v>-45</v>
+      </c>
+      <c r="D135" t="s">
+        <v>18</v>
+      </c>
+      <c r="E135" s="4">
+        <v>42948</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A136">
+        <v>134</v>
+      </c>
+      <c r="B136" t="s">
+        <v>20</v>
+      </c>
+      <c r="C136">
+        <v>-44</v>
+      </c>
+      <c r="D136" t="s">
+        <v>18</v>
+      </c>
+      <c r="E136" s="4">
+        <v>42979</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A137">
+        <v>135</v>
+      </c>
+      <c r="B137" t="s">
+        <v>20</v>
+      </c>
+      <c r="C137">
+        <v>-43</v>
+      </c>
+      <c r="D137" t="s">
+        <v>18</v>
+      </c>
+      <c r="E137" s="4">
+        <v>43009</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A138">
+        <v>136</v>
+      </c>
+      <c r="B138" t="s">
+        <v>20</v>
+      </c>
+      <c r="C138">
+        <v>-42</v>
+      </c>
+      <c r="D138" t="s">
+        <v>18</v>
+      </c>
+      <c r="E138" s="4">
+        <v>43040</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A139">
+        <v>137</v>
+      </c>
+      <c r="B139" t="s">
+        <v>20</v>
+      </c>
+      <c r="C139">
+        <v>-41</v>
+      </c>
+      <c r="D139" t="s">
+        <v>18</v>
+      </c>
+      <c r="E139" s="4">
+        <v>43070</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A140">
+        <v>138</v>
+      </c>
+      <c r="B140" t="s">
+        <v>20</v>
+      </c>
+      <c r="C140">
+        <v>-40</v>
+      </c>
+      <c r="D140" t="s">
+        <v>18</v>
+      </c>
+      <c r="E140" s="4">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A141">
+        <v>139</v>
+      </c>
+      <c r="B141" t="s">
+        <v>20</v>
+      </c>
+      <c r="C141">
+        <v>-39</v>
+      </c>
+      <c r="D141" t="s">
+        <v>18</v>
+      </c>
+      <c r="E141" s="4">
+        <v>43132</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A142">
+        <v>140</v>
+      </c>
+      <c r="B142" t="s">
+        <v>20</v>
+      </c>
+      <c r="C142">
+        <v>-38</v>
+      </c>
+      <c r="D142" t="s">
+        <v>18</v>
+      </c>
+      <c r="E142" s="4">
+        <v>43160</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A143">
+        <v>141</v>
+      </c>
+      <c r="B143" t="s">
+        <v>20</v>
+      </c>
+      <c r="C143">
+        <v>-37</v>
+      </c>
+      <c r="D143" t="s">
+        <v>18</v>
+      </c>
+      <c r="E143" s="4">
+        <v>43191</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A144">
+        <v>142</v>
+      </c>
+      <c r="B144" t="s">
+        <v>21</v>
+      </c>
+      <c r="C144">
+        <v>-52</v>
+      </c>
+      <c r="D144" t="s">
+        <v>18</v>
+      </c>
+      <c r="E144" s="4">
+        <v>42736</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A145">
+        <v>143</v>
+      </c>
+      <c r="B145" t="s">
+        <v>21</v>
+      </c>
+      <c r="C145">
+        <v>-46</v>
+      </c>
+      <c r="D145" t="s">
+        <v>18</v>
+      </c>
+      <c r="E145" s="4">
+        <v>42767</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A146">
+        <v>144</v>
+      </c>
+      <c r="B146" t="s">
+        <v>21</v>
+      </c>
+      <c r="C146">
+        <v>-31</v>
+      </c>
+      <c r="D146" t="s">
+        <v>18</v>
+      </c>
+      <c r="E146" s="4">
+        <v>42795</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A147">
+        <v>145</v>
+      </c>
+      <c r="B147" t="s">
+        <v>21</v>
+      </c>
+      <c r="C147">
+        <v>-40</v>
+      </c>
+      <c r="D147" t="s">
+        <v>18</v>
+      </c>
+      <c r="E147" s="4">
+        <v>42826</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A148">
+        <v>146</v>
+      </c>
+      <c r="B148" t="s">
+        <v>21</v>
+      </c>
+      <c r="C148">
+        <v>-58</v>
+      </c>
+      <c r="D148" t="s">
+        <v>18</v>
+      </c>
+      <c r="E148" s="4">
+        <v>42856</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A149">
+        <v>147</v>
+      </c>
+      <c r="B149" t="s">
+        <v>21</v>
+      </c>
+      <c r="C149">
+        <v>-59</v>
+      </c>
+      <c r="D149" t="s">
+        <v>18</v>
+      </c>
+      <c r="E149" s="4">
+        <v>42887</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A150">
+        <v>148</v>
+      </c>
+      <c r="B150" t="s">
+        <v>21</v>
+      </c>
+      <c r="C150">
+        <v>-59</v>
+      </c>
+      <c r="D150" t="s">
+        <v>18</v>
+      </c>
+      <c r="E150" s="4">
+        <v>42917</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A151">
+        <v>149</v>
+      </c>
+      <c r="B151" t="s">
+        <v>21</v>
+      </c>
+      <c r="C151">
+        <v>-30</v>
+      </c>
+      <c r="D151" t="s">
+        <v>18</v>
+      </c>
+      <c r="E151" s="4">
+        <v>42948</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A152">
+        <v>150</v>
+      </c>
+      <c r="B152" t="s">
+        <v>21</v>
+      </c>
+      <c r="C152">
+        <v>-46</v>
+      </c>
+      <c r="D152" t="s">
+        <v>18</v>
+      </c>
+      <c r="E152" s="4">
+        <v>42979</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A153">
+        <v>151</v>
+      </c>
+      <c r="B153" t="s">
+        <v>21</v>
+      </c>
+      <c r="C153">
+        <v>-56</v>
+      </c>
+      <c r="D153" t="s">
+        <v>18</v>
+      </c>
+      <c r="E153" s="4">
+        <v>43009</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A154">
+        <v>152</v>
+      </c>
+      <c r="B154" t="s">
+        <v>21</v>
+      </c>
+      <c r="C154">
+        <v>-58</v>
+      </c>
+      <c r="D154" t="s">
+        <v>18</v>
+      </c>
+      <c r="E154" s="4">
+        <v>43040</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A155">
+        <v>153</v>
+      </c>
+      <c r="B155" t="s">
+        <v>21</v>
+      </c>
+      <c r="C155">
+        <v>-32</v>
+      </c>
+      <c r="D155" t="s">
+        <v>18</v>
+      </c>
+      <c r="E155" s="4">
+        <v>43070</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A156">
+        <v>154</v>
+      </c>
+      <c r="B156" t="s">
+        <v>21</v>
+      </c>
+      <c r="C156">
+        <v>-56</v>
+      </c>
+      <c r="D156" t="s">
+        <v>18</v>
+      </c>
+      <c r="E156" s="4">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A157">
+        <v>155</v>
+      </c>
+      <c r="B157" t="s">
+        <v>21</v>
+      </c>
+      <c r="C157">
+        <v>-35</v>
+      </c>
+      <c r="D157" t="s">
+        <v>18</v>
+      </c>
+      <c r="E157" s="4">
+        <v>43132</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A158">
+        <v>156</v>
+      </c>
+      <c r="B158" t="s">
+        <v>21</v>
+      </c>
+      <c r="C158">
+        <v>-37</v>
+      </c>
+      <c r="D158" t="s">
+        <v>18</v>
+      </c>
+      <c r="E158" s="4">
+        <v>43160</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A159">
+        <v>157</v>
+      </c>
+      <c r="B159" t="s">
+        <v>21</v>
+      </c>
+      <c r="C159">
+        <v>-51</v>
+      </c>
+      <c r="D159" t="s">
+        <v>18</v>
+      </c>
+      <c r="E159" s="4">
+        <v>43191</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A160">
+        <v>158</v>
+      </c>
+      <c r="B160" t="s">
+        <v>23</v>
+      </c>
+      <c r="C160">
+        <v>-34</v>
+      </c>
+      <c r="D160" t="s">
+        <v>22</v>
+      </c>
+      <c r="E160" s="4">
+        <v>42736</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A161">
+        <v>159</v>
+      </c>
+      <c r="B161" t="s">
+        <v>23</v>
+      </c>
+      <c r="C161">
+        <v>-34</v>
+      </c>
+      <c r="D161" t="s">
+        <v>22</v>
+      </c>
+      <c r="E161" s="4">
+        <v>42767</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A162">
+        <v>160</v>
+      </c>
+      <c r="B162" t="s">
+        <v>23</v>
+      </c>
+      <c r="C162">
+        <v>-34</v>
+      </c>
+      <c r="D162" t="s">
+        <v>22</v>
+      </c>
+      <c r="E162" s="4">
+        <v>42795</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A163">
+        <v>161</v>
+      </c>
+      <c r="B163" t="s">
+        <v>23</v>
+      </c>
+      <c r="C163">
+        <v>-34</v>
+      </c>
+      <c r="D163" t="s">
+        <v>22</v>
+      </c>
+      <c r="E163" s="4">
+        <v>42826</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A164">
+        <v>162</v>
+      </c>
+      <c r="B164" t="s">
+        <v>23</v>
+      </c>
+      <c r="C164">
+        <v>-34</v>
+      </c>
+      <c r="D164" t="s">
+        <v>22</v>
+      </c>
+      <c r="E164" s="4">
+        <v>42856</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A165">
+        <v>163</v>
+      </c>
+      <c r="B165" t="s">
+        <v>23</v>
+      </c>
+      <c r="C165">
+        <v>-34</v>
+      </c>
+      <c r="D165" t="s">
+        <v>22</v>
+      </c>
+      <c r="E165" s="4">
+        <v>42887</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A166">
+        <v>164</v>
+      </c>
+      <c r="B166" t="s">
+        <v>23</v>
+      </c>
+      <c r="C166">
+        <v>-34</v>
+      </c>
+      <c r="D166" t="s">
+        <v>22</v>
+      </c>
+      <c r="E166" s="4">
+        <v>42917</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A167">
+        <v>165</v>
+      </c>
+      <c r="B167" t="s">
+        <v>23</v>
+      </c>
+      <c r="C167">
+        <v>-34</v>
+      </c>
+      <c r="D167" t="s">
+        <v>22</v>
+      </c>
+      <c r="E167" s="4">
+        <v>42948</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A168">
+        <v>166</v>
+      </c>
+      <c r="B168" t="s">
+        <v>23</v>
+      </c>
+      <c r="C168">
+        <v>-34</v>
+      </c>
+      <c r="D168" t="s">
+        <v>22</v>
+      </c>
+      <c r="E168" s="4">
+        <v>42979</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A169">
+        <v>167</v>
+      </c>
+      <c r="B169" t="s">
+        <v>23</v>
+      </c>
+      <c r="C169">
+        <v>-34</v>
+      </c>
+      <c r="D169" t="s">
+        <v>22</v>
+      </c>
+      <c r="E169" s="4">
+        <v>43009</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A170">
+        <v>168</v>
+      </c>
+      <c r="B170" t="s">
+        <v>23</v>
+      </c>
+      <c r="C170">
+        <v>-34</v>
+      </c>
+      <c r="D170" t="s">
+        <v>22</v>
+      </c>
+      <c r="E170" s="4">
+        <v>43040</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A171">
+        <v>169</v>
+      </c>
+      <c r="B171" t="s">
+        <v>23</v>
+      </c>
+      <c r="C171">
+        <v>-34</v>
+      </c>
+      <c r="D171" t="s">
+        <v>22</v>
+      </c>
+      <c r="E171" s="4">
+        <v>43070</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A172">
+        <v>170</v>
+      </c>
+      <c r="B172" t="s">
+        <v>23</v>
+      </c>
+      <c r="C172">
+        <v>-34</v>
+      </c>
+      <c r="D172" t="s">
+        <v>22</v>
+      </c>
+      <c r="E172" s="4">
+        <v>43101</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A173">
+        <v>171</v>
+      </c>
+      <c r="B173" t="s">
+        <v>23</v>
+      </c>
+      <c r="C173">
+        <v>-34</v>
+      </c>
+      <c r="D173" t="s">
+        <v>22</v>
+      </c>
+      <c r="E173" s="4">
+        <v>43132</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A174">
+        <v>172</v>
+      </c>
+      <c r="B174" t="s">
+        <v>23</v>
+      </c>
+      <c r="C174">
+        <v>-34</v>
+      </c>
+      <c r="D174" t="s">
+        <v>22</v>
+      </c>
+      <c r="E174" s="4">
+        <v>43160</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A175">
+        <v>173</v>
+      </c>
+      <c r="B175" t="s">
+        <v>23</v>
+      </c>
+      <c r="C175">
+        <v>-34</v>
+      </c>
+      <c r="D175" t="s">
+        <v>22</v>
+      </c>
+      <c r="E175" s="4">
+        <v>43191</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A176" s="6">
+        <v>174</v>
+      </c>
+      <c r="B176" t="s">
+        <v>24</v>
+      </c>
+      <c r="C176">
+        <v>-30</v>
+      </c>
+      <c r="D176" t="s">
+        <v>22</v>
+      </c>
+      <c r="E176" s="4">
+        <v>42845</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A177" s="6">
+        <v>175</v>
+      </c>
+      <c r="B177" t="s">
+        <v>24</v>
+      </c>
+      <c r="C177">
+        <v>-80</v>
+      </c>
+      <c r="D177" t="s">
+        <v>22</v>
+      </c>
+      <c r="E177" s="4">
+        <v>42920</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A178" s="6">
+        <v>176</v>
+      </c>
+      <c r="B178" t="s">
+        <v>24</v>
+      </c>
+      <c r="C178">
+        <v>-60</v>
+      </c>
+      <c r="D178" t="s">
+        <v>22</v>
+      </c>
+      <c r="E178" s="4">
+        <v>42955</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A179" s="6">
+        <v>177</v>
+      </c>
+      <c r="B179" t="s">
+        <v>24</v>
+      </c>
+      <c r="C179">
+        <v>-20</v>
+      </c>
+      <c r="D179" t="s">
+        <v>22</v>
+      </c>
+      <c r="E179" s="4">
+        <v>43148</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A180" s="6">
+        <v>178</v>
+      </c>
+      <c r="B180" t="s">
+        <v>26</v>
+      </c>
+      <c r="C180">
+        <v>-55</v>
+      </c>
+      <c r="D180" t="s">
+        <v>25</v>
+      </c>
+      <c r="E180" s="4">
+        <v>42755</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A181" s="6">
+        <v>179</v>
+      </c>
+      <c r="B181" t="s">
+        <v>26</v>
+      </c>
+      <c r="C181">
+        <v>-51</v>
+      </c>
+      <c r="D181" t="s">
+        <v>25</v>
+      </c>
+      <c r="E181" s="4">
+        <v>42792</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A182" s="6">
+        <v>180</v>
+      </c>
+      <c r="B182" t="s">
+        <v>26</v>
+      </c>
+      <c r="C182">
+        <v>-75</v>
+      </c>
+      <c r="D182" t="s">
+        <v>25</v>
+      </c>
+      <c r="E182" s="4">
+        <v>42829</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A183" s="6">
+        <v>181</v>
+      </c>
+      <c r="B183" t="s">
+        <v>26</v>
+      </c>
+      <c r="C183">
+        <v>-64</v>
+      </c>
+      <c r="D183" t="s">
+        <v>25</v>
+      </c>
+      <c r="E183" s="4">
+        <v>42860</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A184" s="6">
+        <v>182</v>
+      </c>
+      <c r="B184" t="s">
+        <v>26</v>
+      </c>
+      <c r="C184">
+        <v>-66</v>
+      </c>
+      <c r="D184" t="s">
+        <v>25</v>
+      </c>
+      <c r="E184" s="4">
+        <v>42908</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A185" s="6">
+        <v>183</v>
+      </c>
+      <c r="B185" t="s">
+        <v>26</v>
+      </c>
+      <c r="C185">
+        <v>-59</v>
+      </c>
+      <c r="D185" t="s">
+        <v>25</v>
+      </c>
+      <c r="E185" s="4">
+        <v>42947</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A186" s="6">
+        <v>184</v>
+      </c>
+      <c r="B186" t="s">
+        <v>27</v>
+      </c>
+      <c r="C186">
+        <v>-680</v>
+      </c>
+      <c r="D186" t="s">
+        <v>25</v>
+      </c>
+      <c r="E186" s="4">
+        <v>42975</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A187" s="6">
+        <v>185</v>
+      </c>
+      <c r="B187" t="s">
+        <v>26</v>
+      </c>
+      <c r="C187">
+        <v>-97</v>
+      </c>
+      <c r="D187" t="s">
+        <v>25</v>
+      </c>
+      <c r="E187" s="4">
+        <v>42996</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A188" s="6">
+        <v>186</v>
+      </c>
+      <c r="B188" t="s">
+        <v>26</v>
+      </c>
+      <c r="C188">
+        <v>-56</v>
+      </c>
+      <c r="D188" t="s">
+        <v>25</v>
+      </c>
+      <c r="E188" s="4">
+        <v>43017</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A189" s="6">
+        <v>187</v>
+      </c>
+      <c r="B189" t="s">
+        <v>26</v>
+      </c>
+      <c r="C189">
+        <v>-78</v>
+      </c>
+      <c r="D189" t="s">
+        <v>25</v>
+      </c>
+      <c r="E189" s="4">
+        <v>43065</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A190" s="6">
+        <v>188</v>
+      </c>
+      <c r="B190" t="s">
+        <v>26</v>
+      </c>
+      <c r="C190">
+        <v>-99</v>
+      </c>
+      <c r="D190" t="s">
+        <v>25</v>
+      </c>
+      <c r="E190" s="4">
+        <v>43089</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A191" s="6">
+        <v>189</v>
+      </c>
+      <c r="B191" t="s">
+        <v>26</v>
+      </c>
+      <c r="C191">
+        <v>-53</v>
+      </c>
+      <c r="D191" t="s">
+        <v>25</v>
+      </c>
+      <c r="E191" s="4">
+        <v>43138</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A192" s="6">
+        <v>190</v>
+      </c>
+      <c r="B192" t="s">
+        <v>28</v>
+      </c>
+      <c r="C192">
+        <v>-240</v>
+      </c>
+      <c r="D192" t="s">
+        <v>15</v>
+      </c>
+      <c r="E192" s="4">
+        <v>42769</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A193" s="6">
+        <v>191</v>
+      </c>
+      <c r="B193" t="s">
+        <v>29</v>
+      </c>
+      <c r="C193">
+        <v>-544</v>
+      </c>
+      <c r="D193" t="s">
+        <v>30</v>
+      </c>
+      <c r="E193" s="4">
+        <v>42823</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A194" s="6">
+        <v>192</v>
+      </c>
+      <c r="B194" t="s">
+        <v>31</v>
+      </c>
+      <c r="C194">
+        <v>-200</v>
+      </c>
+      <c r="D194" t="s">
+        <v>30</v>
+      </c>
+      <c r="E194" s="4">
+        <v>42800</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A195" s="6">
+        <v>193</v>
+      </c>
+      <c r="B195" t="s">
+        <v>32</v>
+      </c>
+      <c r="C195">
+        <v>-80</v>
+      </c>
+      <c r="D195" t="s">
+        <v>30</v>
+      </c>
+      <c r="E195" s="4">
+        <v>42831</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A196" s="6">
+        <v>194</v>
+      </c>
+      <c r="B196" t="s">
+        <v>33</v>
+      </c>
+      <c r="C196">
+        <v>-250</v>
+      </c>
+      <c r="D196" t="s">
+        <v>30</v>
+      </c>
+      <c r="E196" s="4">
+        <v>43079</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A197" s="6">
+        <v>195</v>
+      </c>
+      <c r="B197" t="s">
+        <v>34</v>
+      </c>
+      <c r="C197">
+        <v>-450</v>
+      </c>
+      <c r="D197" t="s">
+        <v>15</v>
+      </c>
+      <c r="E197" s="4">
+        <v>43144</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A198" s="6">
+        <v>196</v>
+      </c>
+      <c r="B198" t="s">
+        <v>35</v>
+      </c>
+      <c r="C198">
+        <v>-1500</v>
+      </c>
+      <c r="D198" t="s">
+        <v>30</v>
+      </c>
+      <c r="E198" s="4">
+        <v>42747</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C200" s="5"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E109"/>
+  <autoFilter ref="A1:E110"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
[FIX] Problem with empty rows in data
</commit_message>
<xml_diff>
--- a/sample_data/data.xlsx
+++ b/sample_data/data.xlsx
@@ -139,7 +139,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,14 +149,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -190,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -200,7 +192,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -482,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E200"/>
+  <dimension ref="A1:E198"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="D201" sqref="D201"/>
+      <selection activeCell="A199" sqref="A199:XFD204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3418,7 +3409,7 @@
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A176" s="6">
+      <c r="A176" s="5">
         <v>174</v>
       </c>
       <c r="B176" t="s">
@@ -3435,7 +3426,7 @@
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A177" s="6">
+      <c r="A177" s="5">
         <v>175</v>
       </c>
       <c r="B177" t="s">
@@ -3452,7 +3443,7 @@
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A178" s="6">
+      <c r="A178" s="5">
         <v>176</v>
       </c>
       <c r="B178" t="s">
@@ -3469,7 +3460,7 @@
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A179" s="6">
+      <c r="A179" s="5">
         <v>177</v>
       </c>
       <c r="B179" t="s">
@@ -3486,7 +3477,7 @@
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A180" s="6">
+      <c r="A180" s="5">
         <v>178</v>
       </c>
       <c r="B180" t="s">
@@ -3503,7 +3494,7 @@
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A181" s="6">
+      <c r="A181" s="5">
         <v>179</v>
       </c>
       <c r="B181" t="s">
@@ -3520,7 +3511,7 @@
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A182" s="6">
+      <c r="A182" s="5">
         <v>180</v>
       </c>
       <c r="B182" t="s">
@@ -3537,7 +3528,7 @@
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A183" s="6">
+      <c r="A183" s="5">
         <v>181</v>
       </c>
       <c r="B183" t="s">
@@ -3554,7 +3545,7 @@
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A184" s="6">
+      <c r="A184" s="5">
         <v>182</v>
       </c>
       <c r="B184" t="s">
@@ -3571,7 +3562,7 @@
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A185" s="6">
+      <c r="A185" s="5">
         <v>183</v>
       </c>
       <c r="B185" t="s">
@@ -3588,7 +3579,7 @@
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A186" s="6">
+      <c r="A186" s="5">
         <v>184</v>
       </c>
       <c r="B186" t="s">
@@ -3605,7 +3596,7 @@
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A187" s="6">
+      <c r="A187" s="5">
         <v>185</v>
       </c>
       <c r="B187" t="s">
@@ -3622,7 +3613,7 @@
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A188" s="6">
+      <c r="A188" s="5">
         <v>186</v>
       </c>
       <c r="B188" t="s">
@@ -3639,7 +3630,7 @@
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A189" s="6">
+      <c r="A189" s="5">
         <v>187</v>
       </c>
       <c r="B189" t="s">
@@ -3656,7 +3647,7 @@
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A190" s="6">
+      <c r="A190" s="5">
         <v>188</v>
       </c>
       <c r="B190" t="s">
@@ -3673,7 +3664,7 @@
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A191" s="6">
+      <c r="A191" s="5">
         <v>189</v>
       </c>
       <c r="B191" t="s">
@@ -3690,7 +3681,7 @@
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A192" s="6">
+      <c r="A192" s="5">
         <v>190</v>
       </c>
       <c r="B192" t="s">
@@ -3707,7 +3698,7 @@
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A193" s="6">
+      <c r="A193" s="5">
         <v>191</v>
       </c>
       <c r="B193" t="s">
@@ -3724,7 +3715,7 @@
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A194" s="6">
+      <c r="A194" s="5">
         <v>192</v>
       </c>
       <c r="B194" t="s">
@@ -3741,7 +3732,7 @@
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A195" s="6">
+      <c r="A195" s="5">
         <v>193</v>
       </c>
       <c r="B195" t="s">
@@ -3758,7 +3749,7 @@
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A196" s="6">
+      <c r="A196" s="5">
         <v>194</v>
       </c>
       <c r="B196" t="s">
@@ -3775,7 +3766,7 @@
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A197" s="6">
+      <c r="A197" s="5">
         <v>195</v>
       </c>
       <c r="B197" t="s">
@@ -3792,7 +3783,7 @@
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A198" s="6">
+      <c r="A198" s="5">
         <v>196</v>
       </c>
       <c r="B198" t="s">
@@ -3807,9 +3798,6 @@
       <c r="E198" s="4">
         <v>42747</v>
       </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C200" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E110"/>

</xml_diff>

<commit_message>
[NEW] Add dummy liquid data
</commit_message>
<xml_diff>
--- a/sample_data/data.xlsx
+++ b/sample_data/data.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="trans_m" sheetId="1" r:id="rId1"/>
+    <sheet name="liquid_m" sheetId="3" r:id="rId2"/>
+    <sheet name="liquid_list" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$E$110</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">trans_m!$A$1:$E$110</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="49">
   <si>
     <t>ID</t>
   </si>
@@ -130,14 +132,54 @@
   </si>
   <si>
     <t>Motobike</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Liquidity level</t>
+  </si>
+  <si>
+    <t>Liquidity name</t>
+  </si>
+  <si>
+    <t>Liquid</t>
+  </si>
+  <si>
+    <t>Deposit</t>
+  </si>
+  <si>
+    <t>Potencial investment</t>
+  </si>
+  <si>
+    <t>Robinhood uninvested</t>
+  </si>
+  <si>
+    <t>Bank deposit</t>
+  </si>
+  <si>
+    <t>Personal bank account</t>
+  </si>
+  <si>
+    <t>Shared bank account</t>
+  </si>
+  <si>
+    <t>Fintech account</t>
+  </si>
+  <si>
+    <t>Bank 2 deposit</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="166" formatCode="mm/yyyy"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -182,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -193,6 +235,13 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="A199" sqref="A199:XFD204"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3804,4 +3853,658 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.5546875" style="10"/>
+    <col min="3" max="3" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="8">
+        <v>42736</v>
+      </c>
+      <c r="B2" s="10">
+        <f>SUM(C2:H2)</f>
+        <v>5366</v>
+      </c>
+      <c r="C2">
+        <v>1438</v>
+      </c>
+      <c r="E2">
+        <v>263</v>
+      </c>
+      <c r="G2">
+        <v>2000</v>
+      </c>
+      <c r="H2">
+        <v>1665</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="8">
+        <v>42767</v>
+      </c>
+      <c r="B3" s="10">
+        <f t="shared" ref="B3:B17" si="0">SUM(C3:H3)</f>
+        <v>6238</v>
+      </c>
+      <c r="C3">
+        <v>1341</v>
+      </c>
+      <c r="D3">
+        <v>666</v>
+      </c>
+      <c r="E3">
+        <v>452</v>
+      </c>
+      <c r="G3">
+        <v>2000</v>
+      </c>
+      <c r="H3">
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="8">
+        <v>42795</v>
+      </c>
+      <c r="B4" s="10">
+        <f t="shared" si="0"/>
+        <v>5463</v>
+      </c>
+      <c r="C4">
+        <v>1338</v>
+      </c>
+      <c r="D4">
+        <v>221</v>
+      </c>
+      <c r="E4">
+        <v>469</v>
+      </c>
+      <c r="F4">
+        <v>1000</v>
+      </c>
+      <c r="G4">
+        <v>1000</v>
+      </c>
+      <c r="H4">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
+        <v>42826</v>
+      </c>
+      <c r="B5" s="10">
+        <f t="shared" si="0"/>
+        <v>5850</v>
+      </c>
+      <c r="C5">
+        <v>1432</v>
+      </c>
+      <c r="D5">
+        <v>440</v>
+      </c>
+      <c r="E5">
+        <v>328</v>
+      </c>
+      <c r="F5">
+        <v>1500</v>
+      </c>
+      <c r="G5">
+        <v>1000</v>
+      </c>
+      <c r="H5">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
+        <v>42856</v>
+      </c>
+      <c r="B6" s="10">
+        <f t="shared" si="0"/>
+        <v>6916</v>
+      </c>
+      <c r="C6">
+        <v>1571</v>
+      </c>
+      <c r="D6">
+        <v>878</v>
+      </c>
+      <c r="E6">
+        <v>480</v>
+      </c>
+      <c r="F6">
+        <v>2000</v>
+      </c>
+      <c r="G6">
+        <v>1000</v>
+      </c>
+      <c r="H6">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
+        <v>42887</v>
+      </c>
+      <c r="B7" s="10">
+        <f t="shared" si="0"/>
+        <v>4216</v>
+      </c>
+      <c r="C7">
+        <v>1268</v>
+      </c>
+      <c r="D7">
+        <v>690</v>
+      </c>
+      <c r="E7">
+        <v>435</v>
+      </c>
+      <c r="F7">
+        <v>500</v>
+      </c>
+      <c r="G7">
+        <v>500</v>
+      </c>
+      <c r="H7">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="8">
+        <v>42917</v>
+      </c>
+      <c r="B8" s="10">
+        <f t="shared" si="0"/>
+        <v>3922</v>
+      </c>
+      <c r="C8">
+        <v>1045</v>
+      </c>
+      <c r="D8">
+        <v>646</v>
+      </c>
+      <c r="E8">
+        <v>477</v>
+      </c>
+      <c r="F8">
+        <v>500</v>
+      </c>
+      <c r="G8">
+        <v>500</v>
+      </c>
+      <c r="H8">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
+        <v>42948</v>
+      </c>
+      <c r="B9" s="10">
+        <f t="shared" si="0"/>
+        <v>4575</v>
+      </c>
+      <c r="C9">
+        <v>1178</v>
+      </c>
+      <c r="D9">
+        <v>1144</v>
+      </c>
+      <c r="E9">
+        <v>320</v>
+      </c>
+      <c r="F9">
+        <v>500</v>
+      </c>
+      <c r="G9">
+        <v>500</v>
+      </c>
+      <c r="H9">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="8">
+        <v>42979</v>
+      </c>
+      <c r="B10" s="10">
+        <f t="shared" si="0"/>
+        <v>4943</v>
+      </c>
+      <c r="C10">
+        <v>1423</v>
+      </c>
+      <c r="D10">
+        <v>599</v>
+      </c>
+      <c r="E10">
+        <v>345</v>
+      </c>
+      <c r="F10">
+        <v>1000</v>
+      </c>
+      <c r="G10">
+        <v>500</v>
+      </c>
+      <c r="H10">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
+        <v>43009</v>
+      </c>
+      <c r="B11" s="10">
+        <f t="shared" si="0"/>
+        <v>5852</v>
+      </c>
+      <c r="C11">
+        <v>1589</v>
+      </c>
+      <c r="D11">
+        <v>677</v>
+      </c>
+      <c r="E11">
+        <v>343</v>
+      </c>
+      <c r="F11">
+        <v>1500</v>
+      </c>
+      <c r="G11">
+        <v>500</v>
+      </c>
+      <c r="H11">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="8">
+        <v>43040</v>
+      </c>
+      <c r="B12" s="10">
+        <f t="shared" si="0"/>
+        <v>5984</v>
+      </c>
+      <c r="C12">
+        <v>1337</v>
+      </c>
+      <c r="D12">
+        <v>372</v>
+      </c>
+      <c r="E12">
+        <v>500</v>
+      </c>
+      <c r="F12">
+        <v>2000</v>
+      </c>
+      <c r="G12">
+        <v>500</v>
+      </c>
+      <c r="H12">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="8">
+        <v>43070</v>
+      </c>
+      <c r="B13" s="10">
+        <f t="shared" si="0"/>
+        <v>7801</v>
+      </c>
+      <c r="C13">
+        <v>1374</v>
+      </c>
+      <c r="D13">
+        <v>546</v>
+      </c>
+      <c r="E13">
+        <v>483</v>
+      </c>
+      <c r="F13">
+        <v>2500</v>
+      </c>
+      <c r="G13">
+        <v>1000</v>
+      </c>
+      <c r="H13">
+        <v>1898</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="8">
+        <v>43101</v>
+      </c>
+      <c r="B14" s="10">
+        <f t="shared" si="0"/>
+        <v>7726</v>
+      </c>
+      <c r="C14">
+        <v>1336</v>
+      </c>
+      <c r="D14">
+        <v>307</v>
+      </c>
+      <c r="E14">
+        <v>295</v>
+      </c>
+      <c r="F14">
+        <v>3000</v>
+      </c>
+      <c r="G14">
+        <v>1000</v>
+      </c>
+      <c r="H14">
+        <v>1788</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="8">
+        <v>43132</v>
+      </c>
+      <c r="B15" s="10">
+        <f t="shared" si="0"/>
+        <v>8375</v>
+      </c>
+      <c r="C15">
+        <v>1411</v>
+      </c>
+      <c r="D15">
+        <v>924</v>
+      </c>
+      <c r="E15">
+        <v>382</v>
+      </c>
+      <c r="F15">
+        <v>3500</v>
+      </c>
+      <c r="G15">
+        <v>1000</v>
+      </c>
+      <c r="H15">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="8">
+        <v>43160</v>
+      </c>
+      <c r="B16" s="10">
+        <f t="shared" si="0"/>
+        <v>8670</v>
+      </c>
+      <c r="C16">
+        <v>1540</v>
+      </c>
+      <c r="D16">
+        <v>711</v>
+      </c>
+      <c r="E16">
+        <v>261</v>
+      </c>
+      <c r="F16">
+        <v>4000</v>
+      </c>
+      <c r="G16">
+        <v>1000</v>
+      </c>
+      <c r="H16">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="8">
+        <v>43191</v>
+      </c>
+      <c r="B17" s="10">
+        <f t="shared" si="0"/>
+        <v>10046</v>
+      </c>
+      <c r="C17">
+        <v>1652</v>
+      </c>
+      <c r="D17">
+        <v>941</v>
+      </c>
+      <c r="E17">
+        <v>403</v>
+      </c>
+      <c r="F17">
+        <v>4500</v>
+      </c>
+      <c r="G17">
+        <v>1000</v>
+      </c>
+      <c r="H17">
+        <v>1550</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[NEW] Create a tutorial for the upload page
</commit_message>
<xml_diff>
--- a/sample_data/data.xlsx
+++ b/sample_data/data.xlsx
@@ -179,7 +179,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
-    <numFmt numFmtId="166" formatCode="mm/yyyy"/>
+    <numFmt numFmtId="165" formatCode="mm/yyyy"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -239,7 +239,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -525,7 +525,7 @@
   <dimension ref="A1:E198"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3860,7 +3860,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4417,7 +4417,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4506,5 +4506,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[NEW] categories as a dataframe implemented in every app + sample data updated
</commit_message>
<xml_diff>
--- a/sample_data/data.xlsx
+++ b/sample_data/data.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="trans_m" sheetId="1" r:id="rId1"/>
     <sheet name="liquid_m" sheetId="3" r:id="rId2"/>
     <sheet name="liquid_list" sheetId="4" r:id="rId3"/>
+    <sheet name="categories" sheetId="5" r:id="rId4"/>
+    <sheet name="trans_categ" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">trans_m!$A$1:$E$110</definedName>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="64">
   <si>
     <t>ID</t>
   </si>
@@ -171,6 +173,51 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Color Name</t>
+  </si>
+  <si>
+    <t>Color Index</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>Expenses</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>lime</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Incomes</t>
+  </si>
+  <si>
+    <t>light blue</t>
+  </si>
+  <si>
+    <t>purple</t>
+  </si>
+  <si>
+    <t>grey</t>
   </si>
 </sst>
 </file>
@@ -4416,7 +4463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -4508,4 +4555,219 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2">
+        <v>300</v>
+      </c>
+      <c r="E2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3">
+        <v>300</v>
+      </c>
+      <c r="E3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4">
+        <v>200</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5">
+        <v>500</v>
+      </c>
+      <c r="E5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6">
+        <v>300</v>
+      </c>
+      <c r="E6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7">
+        <v>500</v>
+      </c>
+      <c r="E7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8">
+        <v>300</v>
+      </c>
+      <c r="E8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9">
+        <v>500</v>
+      </c>
+      <c r="E9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10">
+        <v>600</v>
+      </c>
+      <c r="E10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11">
+        <v>200</v>
+      </c>
+      <c r="E11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[REF] only use transactions dataframe
</commit_message>
<xml_diff>
--- a/sample_data/data.xlsx
+++ b/sample_data/data.xlsx
@@ -4,14 +4,10 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="trans_m" sheetId="1" r:id="rId1"/>
-    <sheet name="liquid_m" sheetId="3" r:id="rId2"/>
-    <sheet name="liquid_list" sheetId="4" r:id="rId3"/>
-    <sheet name="categories" sheetId="5" r:id="rId4"/>
-    <sheet name="trans_categ" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">trans_m!$A$1:$E$110</definedName>
@@ -26,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -135,98 +131,13 @@
   <si>
     <t>Motobike</t>
   </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Liquidity level</t>
-  </si>
-  <si>
-    <t>Liquidity name</t>
-  </si>
-  <si>
-    <t>Liquid</t>
-  </si>
-  <si>
-    <t>Deposit</t>
-  </si>
-  <si>
-    <t>Potencial investment</t>
-  </si>
-  <si>
-    <t>Robinhood uninvested</t>
-  </si>
-  <si>
-    <t>Bank deposit</t>
-  </si>
-  <si>
-    <t>Personal bank account</t>
-  </si>
-  <si>
-    <t>Shared bank account</t>
-  </si>
-  <si>
-    <t>Fintech account</t>
-  </si>
-  <si>
-    <t>Bank 2 deposit</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Color Name</t>
-  </si>
-  <si>
-    <t>Color Index</t>
-  </si>
-  <si>
-    <t>Fixed</t>
-  </si>
-  <si>
-    <t>Expenses</t>
-  </si>
-  <si>
-    <t>yellow</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>orange</t>
-  </si>
-  <si>
-    <t>lime</t>
-  </si>
-  <si>
-    <t>green</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>Incomes</t>
-  </si>
-  <si>
-    <t>light blue</t>
-  </si>
-  <si>
-    <t>purple</t>
-  </si>
-  <si>
-    <t>grey</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
-    <numFmt numFmtId="165" formatCode="mm/yyyy"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -271,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -282,13 +193,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E198"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3900,874 +3804,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="11.5546875" style="10"/>
-    <col min="3" max="3" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.21875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="8">
-        <v>42736</v>
-      </c>
-      <c r="B2" s="10">
-        <f>SUM(C2:H2)</f>
-        <v>5366</v>
-      </c>
-      <c r="C2">
-        <v>1438</v>
-      </c>
-      <c r="E2">
-        <v>263</v>
-      </c>
-      <c r="G2">
-        <v>2000</v>
-      </c>
-      <c r="H2">
-        <v>1665</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="8">
-        <v>42767</v>
-      </c>
-      <c r="B3" s="10">
-        <f t="shared" ref="B3:B17" si="0">SUM(C3:H3)</f>
-        <v>6238</v>
-      </c>
-      <c r="C3">
-        <v>1341</v>
-      </c>
-      <c r="D3">
-        <v>666</v>
-      </c>
-      <c r="E3">
-        <v>452</v>
-      </c>
-      <c r="G3">
-        <v>2000</v>
-      </c>
-      <c r="H3">
-        <v>1779</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="8">
-        <v>42795</v>
-      </c>
-      <c r="B4" s="10">
-        <f t="shared" si="0"/>
-        <v>5463</v>
-      </c>
-      <c r="C4">
-        <v>1338</v>
-      </c>
-      <c r="D4">
-        <v>221</v>
-      </c>
-      <c r="E4">
-        <v>469</v>
-      </c>
-      <c r="F4">
-        <v>1000</v>
-      </c>
-      <c r="G4">
-        <v>1000</v>
-      </c>
-      <c r="H4">
-        <v>1435</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="8">
-        <v>42826</v>
-      </c>
-      <c r="B5" s="10">
-        <f t="shared" si="0"/>
-        <v>5850</v>
-      </c>
-      <c r="C5">
-        <v>1432</v>
-      </c>
-      <c r="D5">
-        <v>440</v>
-      </c>
-      <c r="E5">
-        <v>328</v>
-      </c>
-      <c r="F5">
-        <v>1500</v>
-      </c>
-      <c r="G5">
-        <v>1000</v>
-      </c>
-      <c r="H5">
-        <v>1150</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="8">
-        <v>42856</v>
-      </c>
-      <c r="B6" s="10">
-        <f t="shared" si="0"/>
-        <v>6916</v>
-      </c>
-      <c r="C6">
-        <v>1571</v>
-      </c>
-      <c r="D6">
-        <v>878</v>
-      </c>
-      <c r="E6">
-        <v>480</v>
-      </c>
-      <c r="F6">
-        <v>2000</v>
-      </c>
-      <c r="G6">
-        <v>1000</v>
-      </c>
-      <c r="H6">
-        <v>987</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="8">
-        <v>42887</v>
-      </c>
-      <c r="B7" s="10">
-        <f t="shared" si="0"/>
-        <v>4216</v>
-      </c>
-      <c r="C7">
-        <v>1268</v>
-      </c>
-      <c r="D7">
-        <v>690</v>
-      </c>
-      <c r="E7">
-        <v>435</v>
-      </c>
-      <c r="F7">
-        <v>500</v>
-      </c>
-      <c r="G7">
-        <v>500</v>
-      </c>
-      <c r="H7">
-        <v>823</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="8">
-        <v>42917</v>
-      </c>
-      <c r="B8" s="10">
-        <f t="shared" si="0"/>
-        <v>3922</v>
-      </c>
-      <c r="C8">
-        <v>1045</v>
-      </c>
-      <c r="D8">
-        <v>646</v>
-      </c>
-      <c r="E8">
-        <v>477</v>
-      </c>
-      <c r="F8">
-        <v>500</v>
-      </c>
-      <c r="G8">
-        <v>500</v>
-      </c>
-      <c r="H8">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="8">
-        <v>42948</v>
-      </c>
-      <c r="B9" s="10">
-        <f t="shared" si="0"/>
-        <v>4575</v>
-      </c>
-      <c r="C9">
-        <v>1178</v>
-      </c>
-      <c r="D9">
-        <v>1144</v>
-      </c>
-      <c r="E9">
-        <v>320</v>
-      </c>
-      <c r="F9">
-        <v>500</v>
-      </c>
-      <c r="G9">
-        <v>500</v>
-      </c>
-      <c r="H9">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="8">
-        <v>42979</v>
-      </c>
-      <c r="B10" s="10">
-        <f t="shared" si="0"/>
-        <v>4943</v>
-      </c>
-      <c r="C10">
-        <v>1423</v>
-      </c>
-      <c r="D10">
-        <v>599</v>
-      </c>
-      <c r="E10">
-        <v>345</v>
-      </c>
-      <c r="F10">
-        <v>1000</v>
-      </c>
-      <c r="G10">
-        <v>500</v>
-      </c>
-      <c r="H10">
-        <v>1076</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="8">
-        <v>43009</v>
-      </c>
-      <c r="B11" s="10">
-        <f t="shared" si="0"/>
-        <v>5852</v>
-      </c>
-      <c r="C11">
-        <v>1589</v>
-      </c>
-      <c r="D11">
-        <v>677</v>
-      </c>
-      <c r="E11">
-        <v>343</v>
-      </c>
-      <c r="F11">
-        <v>1500</v>
-      </c>
-      <c r="G11">
-        <v>500</v>
-      </c>
-      <c r="H11">
-        <v>1243</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="8">
-        <v>43040</v>
-      </c>
-      <c r="B12" s="10">
-        <f t="shared" si="0"/>
-        <v>5984</v>
-      </c>
-      <c r="C12">
-        <v>1337</v>
-      </c>
-      <c r="D12">
-        <v>372</v>
-      </c>
-      <c r="E12">
-        <v>500</v>
-      </c>
-      <c r="F12">
-        <v>2000</v>
-      </c>
-      <c r="G12">
-        <v>500</v>
-      </c>
-      <c r="H12">
-        <v>1275</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="8">
-        <v>43070</v>
-      </c>
-      <c r="B13" s="10">
-        <f t="shared" si="0"/>
-        <v>7801</v>
-      </c>
-      <c r="C13">
-        <v>1374</v>
-      </c>
-      <c r="D13">
-        <v>546</v>
-      </c>
-      <c r="E13">
-        <v>483</v>
-      </c>
-      <c r="F13">
-        <v>2500</v>
-      </c>
-      <c r="G13">
-        <v>1000</v>
-      </c>
-      <c r="H13">
-        <v>1898</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="8">
-        <v>43101</v>
-      </c>
-      <c r="B14" s="10">
-        <f t="shared" si="0"/>
-        <v>7726</v>
-      </c>
-      <c r="C14">
-        <v>1336</v>
-      </c>
-      <c r="D14">
-        <v>307</v>
-      </c>
-      <c r="E14">
-        <v>295</v>
-      </c>
-      <c r="F14">
-        <v>3000</v>
-      </c>
-      <c r="G14">
-        <v>1000</v>
-      </c>
-      <c r="H14">
-        <v>1788</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="8">
-        <v>43132</v>
-      </c>
-      <c r="B15" s="10">
-        <f t="shared" si="0"/>
-        <v>8375</v>
-      </c>
-      <c r="C15">
-        <v>1411</v>
-      </c>
-      <c r="D15">
-        <v>924</v>
-      </c>
-      <c r="E15">
-        <v>382</v>
-      </c>
-      <c r="F15">
-        <v>3500</v>
-      </c>
-      <c r="G15">
-        <v>1000</v>
-      </c>
-      <c r="H15">
-        <v>1158</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="8">
-        <v>43160</v>
-      </c>
-      <c r="B16" s="10">
-        <f t="shared" si="0"/>
-        <v>8670</v>
-      </c>
-      <c r="C16">
-        <v>1540</v>
-      </c>
-      <c r="D16">
-        <v>711</v>
-      </c>
-      <c r="E16">
-        <v>261</v>
-      </c>
-      <c r="F16">
-        <v>4000</v>
-      </c>
-      <c r="G16">
-        <v>1000</v>
-      </c>
-      <c r="H16">
-        <v>1158</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="8">
-        <v>43191</v>
-      </c>
-      <c r="B17" s="10">
-        <f t="shared" si="0"/>
-        <v>10046</v>
-      </c>
-      <c r="C17">
-        <v>1652</v>
-      </c>
-      <c r="D17">
-        <v>941</v>
-      </c>
-      <c r="E17">
-        <v>403</v>
-      </c>
-      <c r="F17">
-        <v>4500</v>
-      </c>
-      <c r="G17">
-        <v>1000</v>
-      </c>
-      <c r="H17">
-        <v>1550</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B17">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.21875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2">
-        <v>300</v>
-      </c>
-      <c r="E2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3">
-        <v>300</v>
-      </c>
-      <c r="E3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4">
-        <v>200</v>
-      </c>
-      <c r="E4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5">
-        <v>500</v>
-      </c>
-      <c r="E5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6">
-        <v>300</v>
-      </c>
-      <c r="E6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7">
-        <v>500</v>
-      </c>
-      <c r="E7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8">
-        <v>300</v>
-      </c>
-      <c r="E8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D9">
-        <v>500</v>
-      </c>
-      <c r="E9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10">
-        <v>600</v>
-      </c>
-      <c r="E10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11">
-        <v>200</v>
-      </c>
-      <c r="E11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>